<commit_message>
report updates + glossary
</commit_message>
<xml_diff>
--- a/IB/lab6/lab6.xlsx
+++ b/IB/lab6/lab6.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Л 6.2" sheetId="2" r:id="rId1"/>
@@ -292,22 +292,22 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -346,7 +346,7 @@
         <xdr:cNvPr id="3" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{28CE2159-0761-4A9A-B0C1-8727B8C8034C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28CE2159-0761-4A9A-B0C1-8727B8C8034C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -675,7 +675,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -713,7 +713,7 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1">
       <c r="A3" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3">
         <v>290716329017</v>
@@ -736,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -750,54 +750,54 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="24" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="14">
+      <c r="A4" s="12">
         <v>24</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>47050437355283</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>4674517</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>1297633</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>30307619697810</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>330155414629</v>
       </c>
     </row>
@@ -807,13 +807,13 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" t="s">

</xml_diff>